<commit_message>
Finally managed to get write.js to work properly by writing to an excel file. Looks like I'll be using xlsx files after all. Additionally, I converted this project to use Electron so it can run locally on a computer.
</commit_message>
<xml_diff>
--- a/parkingDataTest2.xlsx
+++ b/parkingDataTest2.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -426,10 +426,32 @@
         <v>Dav K</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1" t="str">
+        <v>1/28/2025</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <v>roblox1</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <v>Robert Lox</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="str">
+        <v>1/28/2025</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <v>microsoft2000</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <v>Mike Rowesoft</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>